<commit_message>
Kt6 and 7 were missnamed
</commit_message>
<xml_diff>
--- a/scripts/projects/under_ice/meta_data.xlsx
+++ b/scripts/projects/under_ice/meta_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17540"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28720" windowHeight="16980"/>
   </bookViews>
   <sheets>
     <sheet name="SUMMARY.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="325">
   <si>
     <t>Sample</t>
   </si>
@@ -462,9 +462,6 @@
     <t>LB8</t>
   </si>
   <si>
-    <t>KT6</t>
-  </si>
-  <si>
     <t>Shotgun</t>
   </si>
   <si>
@@ -687,9 +684,6 @@
     <t>kt5</t>
   </si>
   <si>
-    <t>kt6</t>
-  </si>
-  <si>
     <t>kt7</t>
   </si>
   <si>
@@ -997,6 +991,9 @@
   </si>
   <si>
     <t>Volume chosen</t>
+  </si>
+  <si>
+    <t>kt8</t>
   </si>
 </sst>
 </file>
@@ -3042,6 +3039,30 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3052,30 +3073,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3512,10 +3509,10 @@
   <dimension ref="A1:CL43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="BX4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="CD2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AV33" sqref="AV33"/>
+      <selection pane="bottomRight" activeCell="BP38" sqref="BP38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3562,7 +3559,7 @@
         <v>32</v>
       </c>
       <c r="D1" s="221" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>1</v>
@@ -3573,32 +3570,32 @@
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
       <c r="I1" s="233" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="J1" s="10" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="12"/>
       <c r="L1" s="233" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="M1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="N1" s="12"/>
       <c r="O1" s="234" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="P1" s="10" t="s">
         <v>5</v>
       </c>
       <c r="Q1" s="11"/>
       <c r="R1" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S1" s="9"/>
       <c r="T1" s="235" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="U1" s="50" t="s">
         <v>15</v>
@@ -3609,12 +3606,12 @@
       <c r="W1" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="258" t="s">
+      <c r="X1" s="251" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="259"/>
+      <c r="Y1" s="252"/>
       <c r="Z1" s="250" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AA1" s="52" t="s">
         <v>23</v>
@@ -3655,136 +3652,136 @@
       <c r="AR1" s="11"/>
       <c r="AS1" s="11"/>
       <c r="AU1" s="209" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV1" s="216" t="s">
+        <v>159</v>
+      </c>
+      <c r="AW1" s="216" t="s">
         <v>148</v>
       </c>
-      <c r="AV1" s="216" t="s">
-        <v>160</v>
-      </c>
-      <c r="AW1" s="216" t="s">
-        <v>149</v>
-      </c>
       <c r="AX1" s="216" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AY1" s="216" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="AZ1" s="216" t="s">
+        <v>184</v>
+      </c>
+      <c r="BA1" s="216" t="s">
         <v>185</v>
       </c>
-      <c r="BA1" s="216" t="s">
+      <c r="BB1" s="216" t="s">
         <v>186</v>
       </c>
-      <c r="BB1" s="216" t="s">
+      <c r="BC1" s="216" t="s">
         <v>187</v>
       </c>
-      <c r="BC1" s="216" t="s">
+      <c r="BD1" s="216" t="s">
         <v>188</v>
       </c>
-      <c r="BD1" s="216" t="s">
+      <c r="BE1" s="216" t="s">
         <v>189</v>
       </c>
-      <c r="BE1" s="216" t="s">
+      <c r="BF1" s="216" t="s">
         <v>190</v>
       </c>
-      <c r="BF1" s="216" t="s">
+      <c r="BG1" s="216" t="s">
         <v>191</v>
       </c>
-      <c r="BG1" s="216" t="s">
+      <c r="BH1" s="216" t="s">
         <v>192</v>
       </c>
-      <c r="BH1" s="216" t="s">
+      <c r="BI1" s="216" t="s">
         <v>193</v>
       </c>
-      <c r="BI1" s="216" t="s">
+      <c r="BJ1" s="216" t="s">
         <v>194</v>
       </c>
-      <c r="BJ1" s="216" t="s">
+      <c r="BK1" s="216" t="s">
         <v>195</v>
       </c>
-      <c r="BK1" s="216" t="s">
+      <c r="BL1" s="216" t="s">
         <v>196</v>
       </c>
-      <c r="BL1" s="216" t="s">
+      <c r="BM1" s="216" t="s">
         <v>197</v>
       </c>
-      <c r="BM1" s="216" t="s">
+      <c r="BN1" s="216" t="s">
+        <v>312</v>
+      </c>
+      <c r="BO1" s="216" t="s">
         <v>198</v>
       </c>
-      <c r="BN1" s="216" t="s">
-        <v>314</v>
-      </c>
-      <c r="BO1" s="216" t="s">
+      <c r="BP1" s="216" t="s">
         <v>199</v>
       </c>
-      <c r="BP1" s="216" t="s">
-        <v>200</v>
-      </c>
       <c r="BQ1" s="216" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="BR1" s="216" t="s">
+        <v>274</v>
+      </c>
+      <c r="BS1" s="216" t="s">
+        <v>275</v>
+      </c>
+      <c r="BT1" s="216" t="s">
         <v>276</v>
       </c>
-      <c r="BS1" s="216" t="s">
+      <c r="BU1" s="216" t="s">
         <v>277</v>
       </c>
-      <c r="BT1" s="216" t="s">
+      <c r="BV1" s="216" t="s">
         <v>278</v>
       </c>
-      <c r="BU1" s="216" t="s">
+      <c r="BW1" s="216" t="s">
         <v>279</v>
       </c>
-      <c r="BV1" s="216" t="s">
+      <c r="BX1" s="216" t="s">
         <v>280</v>
       </c>
-      <c r="BW1" s="216" t="s">
+      <c r="BY1" s="216" t="s">
         <v>281</v>
       </c>
-      <c r="BX1" s="216" t="s">
+      <c r="BZ1" s="216" t="s">
         <v>282</v>
       </c>
-      <c r="BY1" s="216" t="s">
-        <v>283</v>
-      </c>
-      <c r="BZ1" s="216" t="s">
-        <v>284</v>
-      </c>
       <c r="CA1" s="228" t="s">
+        <v>289</v>
+      </c>
+      <c r="CB1" s="228" t="s">
+        <v>292</v>
+      </c>
+      <c r="CC1" s="228" t="s">
         <v>291</v>
       </c>
-      <c r="CB1" s="228" t="s">
+      <c r="CD1" s="228" t="s">
+        <v>290</v>
+      </c>
+      <c r="CE1" s="231" t="s">
+        <v>308</v>
+      </c>
+      <c r="CF1" s="231" t="s">
+        <v>309</v>
+      </c>
+      <c r="CG1" s="231" t="s">
+        <v>310</v>
+      </c>
+      <c r="CH1" s="229" t="s">
+        <v>293</v>
+      </c>
+      <c r="CI1" s="229" t="s">
         <v>294</v>
       </c>
-      <c r="CC1" s="228" t="s">
-        <v>293</v>
-      </c>
-      <c r="CD1" s="228" t="s">
-        <v>292</v>
-      </c>
-      <c r="CE1" s="231" t="s">
-        <v>310</v>
-      </c>
-      <c r="CF1" s="231" t="s">
-        <v>311</v>
-      </c>
-      <c r="CG1" s="231" t="s">
-        <v>312</v>
-      </c>
-      <c r="CH1" s="229" t="s">
+      <c r="CJ1" s="229" t="s">
         <v>295</v>
       </c>
-      <c r="CI1" s="229" t="s">
+      <c r="CK1" s="230" t="s">
         <v>296</v>
       </c>
-      <c r="CJ1" s="229" t="s">
+      <c r="CL1" s="230" t="s">
         <v>297</v>
-      </c>
-      <c r="CK1" s="230" t="s">
-        <v>298</v>
-      </c>
-      <c r="CL1" s="230" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:90" ht="16" customHeight="1" thickBot="1">
@@ -3856,7 +3853,7 @@
         <v>19</v>
       </c>
       <c r="Z2" s="20" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AA2" s="91" t="s">
         <v>120</v>
@@ -3883,7 +3880,7 @@
         <v>121</v>
       </c>
       <c r="AI2" s="17" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="AJ2" s="80"/>
       <c r="AL2" s="16" t="s">
@@ -4029,7 +4026,7 @@
       <c r="A4" s="33">
         <v>3</v>
       </c>
-      <c r="B4" s="255" t="s">
+      <c r="B4" s="256" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="45">
@@ -4167,7 +4164,7 @@
       <c r="A5" s="34">
         <v>5</v>
       </c>
-      <c r="B5" s="256"/>
+      <c r="B5" s="257"/>
       <c r="C5" s="46">
         <v>2</v>
       </c>
@@ -4303,7 +4300,7 @@
       <c r="A6" s="34">
         <v>7</v>
       </c>
-      <c r="B6" s="257"/>
+      <c r="B6" s="258"/>
       <c r="C6" s="46">
         <v>3</v>
       </c>
@@ -4439,7 +4436,7 @@
       <c r="A7" s="34">
         <v>9</v>
       </c>
-      <c r="B7" s="251"/>
+      <c r="B7" s="259"/>
       <c r="C7" s="46">
         <v>4</v>
       </c>
@@ -4575,7 +4572,7 @@
       <c r="A8" s="34">
         <v>11</v>
       </c>
-      <c r="B8" s="252"/>
+      <c r="B8" s="260"/>
       <c r="C8" s="46">
         <v>5</v>
       </c>
@@ -4711,7 +4708,7 @@
       <c r="A9" s="34">
         <v>13</v>
       </c>
-      <c r="B9" s="252"/>
+      <c r="B9" s="260"/>
       <c r="C9" s="46">
         <v>6</v>
       </c>
@@ -4847,7 +4844,7 @@
       <c r="A10" s="34">
         <v>15</v>
       </c>
-      <c r="B10" s="252"/>
+      <c r="B10" s="260"/>
       <c r="C10" s="46">
         <v>7</v>
       </c>
@@ -4983,7 +4980,7 @@
       <c r="A11" s="35">
         <v>17</v>
       </c>
-      <c r="B11" s="254"/>
+      <c r="B11" s="262"/>
       <c r="C11" s="47">
         <v>8</v>
       </c>
@@ -5119,7 +5116,7 @@
       <c r="A12" s="33">
         <v>19</v>
       </c>
-      <c r="B12" s="260" t="s">
+      <c r="B12" s="253" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="204">
@@ -5255,56 +5252,56 @@
         <v>124</v>
       </c>
       <c r="AV12" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW12" t="s">
+        <v>160</v>
+      </c>
+      <c r="AX12" t="s">
         <v>161</v>
       </c>
-      <c r="AX12" t="s">
-        <v>162</v>
-      </c>
       <c r="AY12" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ12" s="223" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BA12" s="223" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="BB12" s="223"/>
       <c r="BC12" s="223"/>
       <c r="BD12" s="223"/>
       <c r="BE12" s="223"/>
       <c r="BF12" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG12" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH12" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI12" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ12" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG12" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH12" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI12" s="224" t="s">
+      <c r="BK12" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ12" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK12" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL12" s="217" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="BM12" s="218" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="BN12" s="218">
         <v>8</v>
       </c>
       <c r="BO12" s="222" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="BP12" s="219" t="s">
         <v>124</v>
@@ -5313,25 +5310,25 @@
         <v>1</v>
       </c>
       <c r="BR12" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS12" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT12" t="s">
         <v>285</v>
       </c>
-      <c r="BS12" t="s">
+      <c r="BU12" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT12" t="s">
+      <c r="BV12" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU12" s="220" t="s">
+      <c r="BW12" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV12" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW12" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX12" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY12" s="220">
         <v>125</v>
@@ -5340,16 +5337,16 @@
         <v>125</v>
       </c>
       <c r="CA12" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB12" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC12" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD12" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB12" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC12" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD12" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE12" s="232">
         <v>41716</v>
@@ -5361,26 +5358,26 @@
         <v>12.270827000000001</v>
       </c>
       <c r="CH12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="CJ12" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK12" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL12" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:90" ht="15" customHeight="1">
       <c r="A13" s="34">
         <v>21</v>
       </c>
-      <c r="B13" s="261"/>
+      <c r="B13" s="254"/>
       <c r="C13" s="205">
         <v>2</v>
       </c>
@@ -5514,56 +5511,56 @@
         <v>125</v>
       </c>
       <c r="AV13" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AY13" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ13" s="223" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="BA13" s="223" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="BB13" s="223"/>
       <c r="BC13" s="223"/>
       <c r="BD13" s="223"/>
       <c r="BE13" s="223"/>
       <c r="BF13" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG13" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH13" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI13" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ13" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG13" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH13" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI13" s="224" t="s">
+      <c r="BK13" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ13" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK13" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL13" s="217" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="BM13" s="218" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="BN13" s="218">
         <v>8</v>
       </c>
       <c r="BO13" s="222" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="BP13" s="219" t="s">
         <v>125</v>
@@ -5572,25 +5569,25 @@
         <v>2</v>
       </c>
       <c r="BR13" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS13" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT13" t="s">
         <v>285</v>
       </c>
-      <c r="BS13" t="s">
+      <c r="BU13" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT13" t="s">
+      <c r="BV13" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU13" s="220" t="s">
+      <c r="BW13" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV13" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW13" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX13" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY13" s="220">
         <v>125</v>
@@ -5599,16 +5596,16 @@
         <v>125</v>
       </c>
       <c r="CA13" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB13" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC13" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD13" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB13" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC13" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD13" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE13" s="232">
         <v>41716</v>
@@ -5620,26 +5617,26 @@
         <v>12.270827000000001</v>
       </c>
       <c r="CH13" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI13" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="CJ13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK13" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL13" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="1:90" ht="15" customHeight="1">
       <c r="A14" s="34">
         <v>23</v>
       </c>
-      <c r="B14" s="262"/>
+      <c r="B14" s="255"/>
       <c r="C14" s="205">
         <v>3</v>
       </c>
@@ -5771,56 +5768,56 @@
         <v>126</v>
       </c>
       <c r="AV14" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AY14" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ14" s="223" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="BA14" s="223" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="BB14" s="223"/>
       <c r="BC14" s="223"/>
       <c r="BD14" s="223"/>
       <c r="BE14" s="223"/>
       <c r="BF14" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG14" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH14" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI14" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ14" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG14" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH14" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI14" s="224" t="s">
+      <c r="BK14" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ14" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK14" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL14" s="217" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="BM14" s="218" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="BN14" s="218">
         <v>8</v>
       </c>
       <c r="BO14" s="222" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="BP14" s="219" t="s">
         <v>126</v>
@@ -5829,25 +5826,25 @@
         <v>3</v>
       </c>
       <c r="BR14" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS14" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT14" t="s">
         <v>285</v>
       </c>
-      <c r="BS14" t="s">
+      <c r="BU14" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT14" t="s">
+      <c r="BV14" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU14" s="220" t="s">
+      <c r="BW14" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV14" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW14" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX14" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY14" s="220">
         <v>125</v>
@@ -5856,16 +5853,16 @@
         <v>125</v>
       </c>
       <c r="CA14" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB14" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC14" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD14" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB14" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC14" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD14" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE14" s="232">
         <v>41716</v>
@@ -5877,26 +5874,26 @@
         <v>12.270827000000001</v>
       </c>
       <c r="CH14" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI14" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="CJ14" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK14" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL14" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:90" ht="15" customHeight="1">
       <c r="A15" s="34">
         <v>25</v>
       </c>
-      <c r="B15" s="251"/>
+      <c r="B15" s="259"/>
       <c r="C15" s="205">
         <v>4</v>
       </c>
@@ -6030,56 +6027,56 @@
         <v>127</v>
       </c>
       <c r="AV15" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AY15" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ15" s="223" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="BA15" s="223" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="BB15" s="223"/>
       <c r="BC15" s="223"/>
       <c r="BD15" s="223"/>
       <c r="BE15" s="223"/>
       <c r="BF15" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG15" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH15" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI15" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ15" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG15" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH15" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI15" s="224" t="s">
+      <c r="BK15" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ15" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK15" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL15" s="217" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="BM15" s="218" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="BN15" s="218">
         <v>8</v>
       </c>
       <c r="BO15" s="222" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="BP15" s="219" t="s">
         <v>127</v>
@@ -6088,25 +6085,25 @@
         <v>4</v>
       </c>
       <c r="BR15" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS15" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT15" t="s">
         <v>285</v>
       </c>
-      <c r="BS15" t="s">
+      <c r="BU15" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT15" t="s">
+      <c r="BV15" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU15" s="220" t="s">
+      <c r="BW15" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV15" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW15" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX15" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY15" s="220">
         <v>125</v>
@@ -6115,16 +6112,16 @@
         <v>125</v>
       </c>
       <c r="CA15" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB15" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC15" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD15" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB15" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC15" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD15" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE15" s="232">
         <v>41716</v>
@@ -6136,26 +6133,26 @@
         <v>12.270827000000001</v>
       </c>
       <c r="CH15" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI15" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="CJ15" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK15" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL15" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:90" ht="15" customHeight="1">
       <c r="A16" s="34">
         <v>27</v>
       </c>
-      <c r="B16" s="252"/>
+      <c r="B16" s="260"/>
       <c r="C16" s="205">
         <v>5</v>
       </c>
@@ -6289,56 +6286,56 @@
         <v>128</v>
       </c>
       <c r="AV16" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AY16" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ16" s="223" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="BA16" s="223" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="BB16" s="223"/>
       <c r="BC16" s="223"/>
       <c r="BD16" s="223"/>
       <c r="BE16" s="223"/>
       <c r="BF16" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG16" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH16" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI16" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ16" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG16" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH16" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI16" s="224" t="s">
+      <c r="BK16" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ16" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK16" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL16" s="217" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="BM16" s="218" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="BN16" s="218">
         <v>8</v>
       </c>
       <c r="BO16" s="222" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="BP16" s="219" t="s">
         <v>128</v>
@@ -6347,25 +6344,25 @@
         <v>5</v>
       </c>
       <c r="BR16" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS16" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT16" t="s">
         <v>285</v>
       </c>
-      <c r="BS16" t="s">
+      <c r="BU16" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT16" t="s">
+      <c r="BV16" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU16" s="220" t="s">
+      <c r="BW16" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV16" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW16" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX16" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY16" s="220">
         <v>125</v>
@@ -6374,16 +6371,16 @@
         <v>125</v>
       </c>
       <c r="CA16" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB16" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC16" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD16" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB16" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC16" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD16" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE16" s="232">
         <v>41716</v>
@@ -6395,26 +6392,26 @@
         <v>12.270827000000001</v>
       </c>
       <c r="CH16" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI16" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="CJ16" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK16" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL16" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="17" spans="1:90" ht="15" customHeight="1">
       <c r="A17" s="34">
         <v>29</v>
       </c>
-      <c r="B17" s="252"/>
+      <c r="B17" s="260"/>
       <c r="C17" s="205">
         <v>6</v>
       </c>
@@ -6548,56 +6545,56 @@
         <v>129</v>
       </c>
       <c r="AV17" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AY17" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ17" s="223" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="BA17" s="223" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="BB17" s="223"/>
       <c r="BC17" s="223"/>
       <c r="BD17" s="223"/>
       <c r="BE17" s="223"/>
       <c r="BF17" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG17" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH17" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI17" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ17" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG17" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH17" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI17" s="224" t="s">
+      <c r="BK17" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ17" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK17" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL17" s="217" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="BM17" s="218" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="BN17" s="218">
         <v>8</v>
       </c>
       <c r="BO17" s="222" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="BP17" s="219" t="s">
         <v>129</v>
@@ -6606,25 +6603,25 @@
         <v>6</v>
       </c>
       <c r="BR17" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS17" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT17" t="s">
         <v>285</v>
       </c>
-      <c r="BS17" t="s">
+      <c r="BU17" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT17" t="s">
+      <c r="BV17" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU17" s="220" t="s">
+      <c r="BW17" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV17" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW17" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX17" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY17" s="220">
         <v>125</v>
@@ -6633,16 +6630,16 @@
         <v>125</v>
       </c>
       <c r="CA17" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB17" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC17" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD17" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB17" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC17" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD17" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE17" s="232">
         <v>41716</v>
@@ -6654,26 +6651,26 @@
         <v>12.270827000000001</v>
       </c>
       <c r="CH17" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI17" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="CJ17" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK17" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL17" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="18" spans="1:90" ht="15" customHeight="1">
       <c r="A18" s="34">
         <v>31</v>
       </c>
-      <c r="B18" s="252"/>
+      <c r="B18" s="260"/>
       <c r="C18" s="205">
         <v>7</v>
       </c>
@@ -6807,56 +6804,56 @@
         <v>130</v>
       </c>
       <c r="AV18" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AY18" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ18" s="223" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="BA18" s="223" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="BB18" s="223"/>
       <c r="BC18" s="223"/>
       <c r="BD18" s="223"/>
       <c r="BE18" s="223"/>
       <c r="BF18" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG18" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH18" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI18" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ18" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG18" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH18" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI18" s="224" t="s">
+      <c r="BK18" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ18" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK18" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL18" s="217" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="BM18" s="218" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="BN18" s="218">
         <v>8</v>
       </c>
       <c r="BO18" s="222" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="BP18" s="219" t="s">
         <v>130</v>
@@ -6865,25 +6862,25 @@
         <v>7</v>
       </c>
       <c r="BR18" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS18" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT18" t="s">
         <v>285</v>
       </c>
-      <c r="BS18" t="s">
+      <c r="BU18" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT18" t="s">
+      <c r="BV18" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU18" s="220" t="s">
+      <c r="BW18" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV18" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW18" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX18" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY18" s="220">
         <v>125</v>
@@ -6892,16 +6889,16 @@
         <v>125</v>
       </c>
       <c r="CA18" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB18" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC18" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD18" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB18" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC18" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD18" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE18" s="232">
         <v>41716</v>
@@ -6913,26 +6910,26 @@
         <v>12.270827000000001</v>
       </c>
       <c r="CH18" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI18" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="CJ18" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK18" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL18" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="19" spans="1:90" ht="16" customHeight="1" thickBot="1">
       <c r="A19" s="35">
         <v>33</v>
       </c>
-      <c r="B19" s="254"/>
+      <c r="B19" s="262"/>
       <c r="C19" s="206">
         <v>8</v>
       </c>
@@ -7066,56 +7063,56 @@
         <v>131</v>
       </c>
       <c r="AV19" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AY19" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ19" s="223" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="BA19" s="223" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="BB19" s="223"/>
       <c r="BC19" s="223"/>
       <c r="BD19" s="223"/>
       <c r="BE19" s="223"/>
       <c r="BF19" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG19" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH19" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI19" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ19" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG19" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH19" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI19" s="224" t="s">
+      <c r="BK19" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ19" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK19" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL19" s="217" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="BM19" s="218" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="BN19" s="218">
         <v>8</v>
       </c>
       <c r="BO19" s="222" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="BP19" s="219" t="s">
         <v>131</v>
@@ -7124,25 +7121,25 @@
         <v>8</v>
       </c>
       <c r="BR19" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS19" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT19" t="s">
         <v>285</v>
       </c>
-      <c r="BS19" t="s">
+      <c r="BU19" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT19" t="s">
+      <c r="BV19" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU19" s="220" t="s">
+      <c r="BW19" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV19" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW19" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX19" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY19" s="220">
         <v>125</v>
@@ -7151,16 +7148,16 @@
         <v>125</v>
       </c>
       <c r="CA19" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB19" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC19" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD19" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB19" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC19" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD19" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE19" s="232">
         <v>41717</v>
@@ -7172,26 +7169,26 @@
         <v>12.270827000000001</v>
       </c>
       <c r="CH19" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI19" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="CJ19" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK19" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL19" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="20" spans="1:90" ht="16" thickTop="1">
       <c r="A20" s="33">
         <v>35</v>
       </c>
-      <c r="B20" s="255" t="s">
+      <c r="B20" s="256" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="204">
@@ -7327,56 +7324,56 @@
         <v>139</v>
       </c>
       <c r="AV20" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AY20" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ20" s="223" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="BA20" s="223" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="BB20" s="223"/>
       <c r="BC20" s="223"/>
       <c r="BD20" s="223"/>
       <c r="BE20" s="223"/>
       <c r="BF20" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG20" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH20" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI20" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ20" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG20" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH20" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI20" s="224" t="s">
+      <c r="BK20" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ20" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK20" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL20" s="217" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BM20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BN20" s="218">
         <v>8</v>
       </c>
       <c r="BO20" s="222" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="BP20" s="219" t="s">
         <v>139</v>
@@ -7385,25 +7382,25 @@
         <v>1</v>
       </c>
       <c r="BR20" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS20" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT20" t="s">
         <v>285</v>
       </c>
-      <c r="BS20" t="s">
+      <c r="BU20" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT20" t="s">
+      <c r="BV20" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU20" s="220" t="s">
+      <c r="BW20" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV20" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW20" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX20" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY20" s="220">
         <v>125</v>
@@ -7412,16 +7409,16 @@
         <v>125</v>
       </c>
       <c r="CA20" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB20" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC20" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD20" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB20" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC20" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD20" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE20" s="232">
         <v>41717</v>
@@ -7433,26 +7430,26 @@
         <v>12.548028</v>
       </c>
       <c r="CH20" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI20" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="CJ20" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK20" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL20" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="21" spans="1:90">
       <c r="A21" s="34">
         <v>37</v>
       </c>
-      <c r="B21" s="256"/>
+      <c r="B21" s="257"/>
       <c r="C21" s="207">
         <v>2</v>
       </c>
@@ -7586,56 +7583,56 @@
         <v>140</v>
       </c>
       <c r="AV21" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AY21" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ21" s="223" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="BA21" s="223" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="BB21" s="223"/>
       <c r="BC21" s="223"/>
       <c r="BD21" s="223"/>
       <c r="BE21" s="223"/>
       <c r="BF21" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG21" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH21" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI21" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ21" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG21" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH21" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI21" s="224" t="s">
+      <c r="BK21" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ21" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK21" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL21" s="217" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BM21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BN21" s="218">
         <v>8</v>
       </c>
       <c r="BO21" s="222" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="BP21" s="219" t="s">
         <v>140</v>
@@ -7644,25 +7641,25 @@
         <v>2</v>
       </c>
       <c r="BR21" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS21" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT21" t="s">
         <v>285</v>
       </c>
-      <c r="BS21" t="s">
+      <c r="BU21" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT21" t="s">
+      <c r="BV21" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU21" s="220" t="s">
+      <c r="BW21" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV21" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW21" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX21" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY21" s="220">
         <v>125</v>
@@ -7671,16 +7668,16 @@
         <v>125</v>
       </c>
       <c r="CA21" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB21" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC21" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD21" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB21" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC21" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD21" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE21" s="232">
         <v>41717</v>
@@ -7692,26 +7689,26 @@
         <v>12.548028</v>
       </c>
       <c r="CH21" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="CJ21" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK21" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL21" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="22" spans="1:90">
       <c r="A22" s="34">
         <v>39</v>
       </c>
-      <c r="B22" s="257"/>
+      <c r="B22" s="258"/>
       <c r="C22" s="207">
         <v>3</v>
       </c>
@@ -7845,56 +7842,56 @@
         <v>141</v>
       </c>
       <c r="AV22" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AY22" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ22" s="223" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="BA22" s="223" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="BB22" s="223"/>
       <c r="BC22" s="223"/>
       <c r="BD22" s="223"/>
       <c r="BE22" s="223"/>
       <c r="BF22" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG22" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH22" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI22" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ22" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG22" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH22" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI22" s="224" t="s">
+      <c r="BK22" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ22" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK22" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL22" s="217" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BM22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BN22" s="218">
         <v>8</v>
       </c>
       <c r="BO22" s="222" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="BP22" s="219" t="s">
         <v>141</v>
@@ -7903,25 +7900,25 @@
         <v>3</v>
       </c>
       <c r="BR22" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS22" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT22" t="s">
         <v>285</v>
       </c>
-      <c r="BS22" t="s">
+      <c r="BU22" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT22" t="s">
+      <c r="BV22" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU22" s="220" t="s">
+      <c r="BW22" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV22" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW22" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX22" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY22" s="220">
         <v>125</v>
@@ -7930,16 +7927,16 @@
         <v>125</v>
       </c>
       <c r="CA22" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB22" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC22" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD22" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB22" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC22" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD22" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE22" s="232">
         <v>41717</v>
@@ -7951,26 +7948,26 @@
         <v>12.548028</v>
       </c>
       <c r="CH22" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI22" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="CJ22" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK22" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL22" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="23" spans="1:90">
       <c r="A23" s="34">
         <v>41</v>
       </c>
-      <c r="B23" s="251"/>
+      <c r="B23" s="259"/>
       <c r="C23" s="205">
         <v>4</v>
       </c>
@@ -8104,56 +8101,56 @@
         <v>142</v>
       </c>
       <c r="AV23" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AY23" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ23" s="223" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="BA23" s="223" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="BB23" s="223"/>
       <c r="BC23" s="223"/>
       <c r="BD23" s="223"/>
       <c r="BE23" s="223"/>
       <c r="BF23" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG23" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH23" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI23" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ23" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG23" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH23" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI23" s="224" t="s">
+      <c r="BK23" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ23" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK23" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL23" s="217" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BM23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BN23" s="218">
         <v>8</v>
       </c>
       <c r="BO23" s="222" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="BP23" s="219" t="s">
         <v>142</v>
@@ -8162,25 +8159,25 @@
         <v>4</v>
       </c>
       <c r="BR23" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS23" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT23" t="s">
         <v>285</v>
       </c>
-      <c r="BS23" t="s">
+      <c r="BU23" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT23" t="s">
+      <c r="BV23" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU23" s="220" t="s">
+      <c r="BW23" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV23" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW23" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX23" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY23" s="220">
         <v>125</v>
@@ -8189,16 +8186,16 @@
         <v>125</v>
       </c>
       <c r="CA23" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB23" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC23" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD23" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB23" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC23" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD23" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE23" s="232">
         <v>41717</v>
@@ -8210,26 +8207,26 @@
         <v>12.548028</v>
       </c>
       <c r="CH23" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI23" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="CJ23" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK23" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL23" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="24" spans="1:90">
       <c r="A24" s="34">
         <v>43</v>
       </c>
-      <c r="B24" s="252"/>
+      <c r="B24" s="260"/>
       <c r="C24" s="205">
         <v>5</v>
       </c>
@@ -8363,56 +8360,56 @@
         <v>143</v>
       </c>
       <c r="AV24" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AY24" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ24" s="223" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="BA24" s="223" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="BB24" s="223"/>
       <c r="BC24" s="223"/>
       <c r="BD24" s="223"/>
       <c r="BE24" s="223"/>
       <c r="BF24" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG24" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH24" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI24" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ24" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG24" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH24" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI24" s="224" t="s">
+      <c r="BK24" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ24" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK24" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL24" s="217" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BM24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BN24" s="218">
         <v>8</v>
       </c>
       <c r="BO24" s="222" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="BP24" s="219" t="s">
         <v>143</v>
@@ -8421,25 +8418,25 @@
         <v>5</v>
       </c>
       <c r="BR24" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS24" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT24" t="s">
         <v>285</v>
       </c>
-      <c r="BS24" t="s">
+      <c r="BU24" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT24" t="s">
+      <c r="BV24" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU24" s="220" t="s">
+      <c r="BW24" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV24" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW24" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX24" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY24" s="220">
         <v>125</v>
@@ -8448,16 +8445,16 @@
         <v>125</v>
       </c>
       <c r="CA24" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB24" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC24" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD24" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB24" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC24" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD24" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE24" s="232">
         <v>41717</v>
@@ -8469,26 +8466,26 @@
         <v>12.548028</v>
       </c>
       <c r="CH24" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI24" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="CJ24" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK24" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL24" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="25" spans="1:90">
       <c r="A25" s="34">
         <v>45</v>
       </c>
-      <c r="B25" s="252"/>
+      <c r="B25" s="260"/>
       <c r="C25" s="205">
         <v>6</v>
       </c>
@@ -8622,56 +8619,56 @@
         <v>144</v>
       </c>
       <c r="AV25" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AY25" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ25" s="223" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="BA25" s="223" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="BB25" s="223"/>
       <c r="BC25" s="223"/>
       <c r="BD25" s="223"/>
       <c r="BE25" s="223"/>
       <c r="BF25" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG25" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH25" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI25" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ25" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG25" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH25" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI25" s="224" t="s">
+      <c r="BK25" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ25" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK25" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL25" s="217" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BM25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BN25" s="218">
         <v>8</v>
       </c>
       <c r="BO25" s="222" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="BP25" s="219" t="s">
         <v>144</v>
@@ -8680,25 +8677,25 @@
         <v>6</v>
       </c>
       <c r="BR25" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS25" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT25" t="s">
         <v>285</v>
       </c>
-      <c r="BS25" t="s">
+      <c r="BU25" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT25" t="s">
+      <c r="BV25" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU25" s="220" t="s">
+      <c r="BW25" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV25" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW25" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX25" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY25" s="220">
         <v>125</v>
@@ -8707,16 +8704,16 @@
         <v>125</v>
       </c>
       <c r="CA25" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB25" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC25" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD25" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB25" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC25" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD25" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE25" s="232">
         <v>41717</v>
@@ -8728,26 +8725,26 @@
         <v>12.548028</v>
       </c>
       <c r="CH25" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI25" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="CJ25" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK25" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL25" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="26" spans="1:90">
       <c r="A26" s="34">
         <v>47</v>
       </c>
-      <c r="B26" s="252"/>
+      <c r="B26" s="260"/>
       <c r="C26" s="205">
         <v>7</v>
       </c>
@@ -8885,56 +8882,56 @@
         <v>145</v>
       </c>
       <c r="AV26" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX26" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AY26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ26" s="223" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="BA26" s="223" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="BB26" s="223"/>
       <c r="BC26" s="223"/>
       <c r="BD26" s="223"/>
       <c r="BE26" s="223"/>
       <c r="BF26" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG26" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH26" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI26" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ26" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG26" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH26" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI26" s="224" t="s">
+      <c r="BK26" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ26" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK26" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL26" s="217" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BM26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BN26" s="218">
         <v>8</v>
       </c>
       <c r="BO26" s="222" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="BP26" s="219" t="s">
         <v>145</v>
@@ -8943,25 +8940,25 @@
         <v>7</v>
       </c>
       <c r="BR26" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS26" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT26" t="s">
         <v>285</v>
       </c>
-      <c r="BS26" t="s">
+      <c r="BU26" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT26" t="s">
+      <c r="BV26" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU26" s="220" t="s">
+      <c r="BW26" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV26" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW26" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX26" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY26" s="220">
         <v>125</v>
@@ -8970,16 +8967,16 @@
         <v>125</v>
       </c>
       <c r="CA26" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB26" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC26" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD26" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB26" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC26" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD26" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE26" s="232">
         <v>41717</v>
@@ -8991,26 +8988,26 @@
         <v>12.548028</v>
       </c>
       <c r="CH26" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="CJ26" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK26" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL26" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="27" spans="1:90" ht="16" thickBot="1">
       <c r="A27" s="35">
         <v>49</v>
       </c>
-      <c r="B27" s="254"/>
+      <c r="B27" s="262"/>
       <c r="C27" s="206">
         <v>8</v>
       </c>
@@ -9148,56 +9145,56 @@
         <v>146</v>
       </c>
       <c r="AV27" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AY27" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ27" s="223" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="BA27" s="223" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="BB27" s="223"/>
       <c r="BC27" s="223"/>
       <c r="BD27" s="223"/>
       <c r="BE27" s="223"/>
       <c r="BF27" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG27" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH27" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI27" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ27" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG27" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH27" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI27" s="224" t="s">
+      <c r="BK27" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ27" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK27" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL27" s="217" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BM27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BN27" s="218">
         <v>8</v>
       </c>
       <c r="BO27" s="222" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="BP27" s="219" t="s">
         <v>146</v>
@@ -9206,25 +9203,25 @@
         <v>8</v>
       </c>
       <c r="BR27" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS27" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT27" t="s">
         <v>285</v>
       </c>
-      <c r="BS27" t="s">
+      <c r="BU27" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT27" t="s">
+      <c r="BV27" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU27" s="220" t="s">
+      <c r="BW27" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV27" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW27" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX27" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY27" s="220">
         <v>125</v>
@@ -9233,16 +9230,16 @@
         <v>125</v>
       </c>
       <c r="CA27" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB27" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC27" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD27" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB27" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC27" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD27" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE27" s="232">
         <v>41718</v>
@@ -9254,26 +9251,26 @@
         <v>12.548028</v>
       </c>
       <c r="CH27" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI27" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="CJ27" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK27" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL27" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="28" spans="1:90" ht="16" thickTop="1">
       <c r="A28" s="33">
         <v>51</v>
       </c>
-      <c r="B28" s="255" t="s">
+      <c r="B28" s="256" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="204">
@@ -9407,56 +9404,56 @@
         <v>132</v>
       </c>
       <c r="AV28" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW28" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AY28" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ28" s="223" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="BA28" s="223" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="BB28" s="223"/>
       <c r="BC28" s="223"/>
       <c r="BD28" s="223"/>
       <c r="BE28" s="223"/>
       <c r="BF28" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG28" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH28" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI28" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ28" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG28" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH28" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI28" s="224" t="s">
+      <c r="BK28" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ28" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK28" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL28" s="217" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BM28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="BN28" s="218">
         <v>8</v>
       </c>
       <c r="BO28" s="222" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="BP28" s="219" t="s">
         <v>132</v>
@@ -9465,25 +9462,25 @@
         <v>1</v>
       </c>
       <c r="BR28" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS28" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT28" t="s">
         <v>285</v>
       </c>
-      <c r="BS28" t="s">
+      <c r="BU28" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT28" t="s">
+      <c r="BV28" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU28" s="220" t="s">
+      <c r="BW28" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV28" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW28" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX28" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY28" s="220">
         <v>125</v>
@@ -9492,16 +9489,16 @@
         <v>125</v>
       </c>
       <c r="CA28" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB28" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC28" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD28" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB28" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC28" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD28" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE28" s="232">
         <v>41718</v>
@@ -9513,26 +9510,26 @@
         <v>14.458780000000001</v>
       </c>
       <c r="CH28" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI28" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="CJ28" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK28" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL28" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="29" spans="1:90">
       <c r="A29" s="34">
         <v>53</v>
       </c>
-      <c r="B29" s="256"/>
+      <c r="B29" s="257"/>
       <c r="C29" s="205">
         <v>2</v>
       </c>
@@ -9664,56 +9661,56 @@
         <v>133</v>
       </c>
       <c r="AV29" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AY29" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ29" s="223" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="BA29" s="223" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="BB29" s="223"/>
       <c r="BC29" s="223"/>
       <c r="BD29" s="223"/>
       <c r="BE29" s="223"/>
       <c r="BF29" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG29" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH29" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI29" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ29" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG29" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH29" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI29" s="224" t="s">
+      <c r="BK29" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ29" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK29" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL29" s="217" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BM29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="BN29" s="218">
         <v>8</v>
       </c>
       <c r="BO29" s="222" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="BP29" s="219" t="s">
         <v>133</v>
@@ -9722,25 +9719,25 @@
         <v>2</v>
       </c>
       <c r="BR29" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS29" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT29" t="s">
         <v>285</v>
       </c>
-      <c r="BS29" t="s">
+      <c r="BU29" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT29" t="s">
+      <c r="BV29" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU29" s="220" t="s">
+      <c r="BW29" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV29" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW29" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX29" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY29" s="220">
         <v>125</v>
@@ -9749,16 +9746,16 @@
         <v>125</v>
       </c>
       <c r="CA29" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB29" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC29" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD29" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB29" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC29" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD29" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE29" s="232">
         <v>41718</v>
@@ -9770,26 +9767,26 @@
         <v>14.458780000000001</v>
       </c>
       <c r="CH29" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI29" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="CJ29" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK29" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL29" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="30" spans="1:90">
       <c r="A30" s="34">
         <v>55</v>
       </c>
-      <c r="B30" s="257"/>
+      <c r="B30" s="258"/>
       <c r="C30" s="205">
         <v>3</v>
       </c>
@@ -9921,56 +9918,56 @@
         <v>134</v>
       </c>
       <c r="AV30" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AY30" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ30" s="223" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="BA30" s="223" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="BB30" s="223"/>
       <c r="BC30" s="223"/>
       <c r="BD30" s="223"/>
       <c r="BE30" s="223"/>
       <c r="BF30" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG30" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH30" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI30" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ30" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG30" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH30" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI30" s="224" t="s">
+      <c r="BK30" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ30" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK30" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL30" s="217" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BM30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="BN30" s="218">
         <v>8</v>
       </c>
       <c r="BO30" s="222" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="BP30" s="219" t="s">
         <v>134</v>
@@ -9979,25 +9976,25 @@
         <v>3</v>
       </c>
       <c r="BR30" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS30" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT30" t="s">
         <v>285</v>
       </c>
-      <c r="BS30" t="s">
+      <c r="BU30" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT30" t="s">
+      <c r="BV30" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU30" s="220" t="s">
+      <c r="BW30" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV30" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW30" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX30" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY30" s="220">
         <v>125</v>
@@ -10006,16 +10003,16 @@
         <v>125</v>
       </c>
       <c r="CA30" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB30" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC30" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD30" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB30" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC30" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD30" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE30" s="232">
         <v>41718</v>
@@ -10027,26 +10024,26 @@
         <v>14.458780000000001</v>
       </c>
       <c r="CH30" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI30" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="CJ30" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK30" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL30" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="31" spans="1:90">
       <c r="A31" s="34">
         <v>57</v>
       </c>
-      <c r="B31" s="251"/>
+      <c r="B31" s="259"/>
       <c r="C31" s="205">
         <v>4</v>
       </c>
@@ -10178,56 +10175,56 @@
         <v>135</v>
       </c>
       <c r="AV31" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AY31" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ31" s="223" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="BA31" s="223" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="BB31" s="223"/>
       <c r="BC31" s="223"/>
       <c r="BD31" s="223"/>
       <c r="BE31" s="223"/>
       <c r="BF31" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG31" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH31" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI31" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ31" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG31" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH31" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI31" s="224" t="s">
+      <c r="BK31" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ31" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK31" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL31" s="217" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BM31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="BN31" s="218">
         <v>8</v>
       </c>
       <c r="BO31" s="222" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="BP31" s="219" t="s">
         <v>135</v>
@@ -10236,25 +10233,25 @@
         <v>4</v>
       </c>
       <c r="BR31" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS31" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT31" t="s">
         <v>285</v>
       </c>
-      <c r="BS31" t="s">
+      <c r="BU31" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT31" t="s">
+      <c r="BV31" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU31" s="220" t="s">
+      <c r="BW31" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV31" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW31" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX31" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY31" s="220">
         <v>125</v>
@@ -10263,16 +10260,16 @@
         <v>125</v>
       </c>
       <c r="CA31" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB31" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC31" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD31" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB31" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC31" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD31" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE31" s="232">
         <v>41718</v>
@@ -10284,26 +10281,26 @@
         <v>14.458780000000001</v>
       </c>
       <c r="CH31" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI31" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="CJ31" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK31" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL31" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="32" spans="1:90">
       <c r="A32" s="34">
         <v>59</v>
       </c>
-      <c r="B32" s="252"/>
+      <c r="B32" s="260"/>
       <c r="C32" s="205">
         <v>5</v>
       </c>
@@ -10435,56 +10432,56 @@
         <v>136</v>
       </c>
       <c r="AV32" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX32" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AY32" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ32" s="223" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="BA32" s="223" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="BB32" s="223"/>
       <c r="BC32" s="223"/>
       <c r="BD32" s="223"/>
       <c r="BE32" s="223"/>
       <c r="BF32" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG32" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH32" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI32" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ32" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG32" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH32" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI32" s="224" t="s">
+      <c r="BK32" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ32" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK32" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL32" s="217" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BM32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="BN32" s="218">
         <v>8</v>
       </c>
       <c r="BO32" s="222" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="BP32" s="219" t="s">
         <v>136</v>
@@ -10493,25 +10490,25 @@
         <v>5</v>
       </c>
       <c r="BR32" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS32" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT32" t="s">
         <v>285</v>
       </c>
-      <c r="BS32" t="s">
+      <c r="BU32" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT32" t="s">
+      <c r="BV32" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU32" s="220" t="s">
+      <c r="BW32" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV32" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW32" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX32" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY32" s="220">
         <v>125</v>
@@ -10520,16 +10517,16 @@
         <v>125</v>
       </c>
       <c r="CA32" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB32" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC32" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD32" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB32" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC32" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD32" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE32" s="232">
         <v>41718</v>
@@ -10541,26 +10538,26 @@
         <v>14.458780000000001</v>
       </c>
       <c r="CH32" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI32" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="CJ32" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK32" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL32" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="33" spans="1:90">
       <c r="A33" s="34">
         <v>61</v>
       </c>
-      <c r="B33" s="252"/>
+      <c r="B33" s="260"/>
       <c r="C33" s="205">
         <v>6</v>
       </c>
@@ -10727,7 +10724,7 @@
       <c r="A34" s="34">
         <v>63</v>
       </c>
-      <c r="B34" s="252"/>
+      <c r="B34" s="260"/>
       <c r="C34" s="205">
         <v>7</v>
       </c>
@@ -10859,83 +10856,83 @@
         <v>137</v>
       </c>
       <c r="AV34" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX34" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AY34" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ34" s="223" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="BA34" s="223" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="BB34" s="223"/>
       <c r="BC34" s="223"/>
       <c r="BD34" s="223"/>
       <c r="BE34" s="223"/>
       <c r="BF34" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG34" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH34" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI34" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ34" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG34" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH34" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI34" s="224" t="s">
+      <c r="BK34" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ34" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK34" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL34" s="217" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BM34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="BN34" s="218">
         <v>8</v>
       </c>
       <c r="BO34" s="222" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="BP34" s="219" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="BQ34" s="222">
         <v>6</v>
       </c>
       <c r="BR34" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS34" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT34" t="s">
         <v>285</v>
       </c>
-      <c r="BS34" t="s">
+      <c r="BU34" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT34" t="s">
+      <c r="BV34" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU34" s="220" t="s">
+      <c r="BW34" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV34" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW34" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX34" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY34" s="220">
         <v>125</v>
@@ -10944,16 +10941,16 @@
         <v>125</v>
       </c>
       <c r="CA34" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB34" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC34" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD34" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB34" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC34" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD34" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE34" s="232">
         <v>41718</v>
@@ -10965,26 +10962,26 @@
         <v>14.458780000000001</v>
       </c>
       <c r="CH34" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI34" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="CJ34" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK34" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL34" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="35" spans="1:90" ht="16" thickBot="1">
       <c r="A35" s="35">
         <v>65</v>
       </c>
-      <c r="B35" s="254"/>
+      <c r="B35" s="262"/>
       <c r="C35" s="206">
         <v>8</v>
       </c>
@@ -11116,83 +11113,83 @@
         <v>138</v>
       </c>
       <c r="AV35" s="219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW35" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AY35" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AZ35" s="223" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="BA35" s="223" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="BB35" s="223"/>
       <c r="BC35" s="223"/>
       <c r="BD35" s="223"/>
       <c r="BE35" s="223"/>
       <c r="BF35" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG35" s="225" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH35" s="226" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI35" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="BJ35" s="225" t="s">
         <v>272</v>
       </c>
-      <c r="BG35" s="225" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH35" s="226" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI35" s="224" t="s">
+      <c r="BK35" s="227" t="s">
         <v>273</v>
       </c>
-      <c r="BJ35" s="225" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK35" s="227" t="s">
-        <v>275</v>
-      </c>
       <c r="BL35" s="217" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BM35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="BN35" s="218">
         <v>8</v>
       </c>
       <c r="BO35" s="222" t="s">
-        <v>223</v>
+        <v>324</v>
       </c>
       <c r="BP35" s="219" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BQ35" s="222">
         <v>7</v>
       </c>
       <c r="BR35" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS35" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT35" t="s">
         <v>285</v>
       </c>
-      <c r="BS35" t="s">
+      <c r="BU35" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="BT35" t="s">
+      <c r="BV35" s="220" t="s">
         <v>287</v>
       </c>
-      <c r="BU35" s="220" t="s">
+      <c r="BW35" s="220" t="s">
         <v>288</v>
       </c>
-      <c r="BV35" s="220" t="s">
-        <v>289</v>
-      </c>
-      <c r="BW35" s="220" t="s">
-        <v>290</v>
-      </c>
       <c r="BX35" s="220" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BY35" s="220">
         <v>125</v>
@@ -11201,16 +11198,16 @@
         <v>125</v>
       </c>
       <c r="CA35" s="220" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB35" s="220" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC35" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="CD35" s="220" t="s">
         <v>305</v>
-      </c>
-      <c r="CB35" s="220" t="s">
-        <v>306</v>
-      </c>
-      <c r="CC35" s="220" t="s">
-        <v>308</v>
-      </c>
-      <c r="CD35" s="220" t="s">
-        <v>307</v>
       </c>
       <c r="CE35" s="232">
         <v>41718</v>
@@ -11222,26 +11219,26 @@
         <v>14.458780000000001</v>
       </c>
       <c r="CH35" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="CI35" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="CJ35" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="CK35" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="CL35" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="36" spans="1:90" ht="16" thickTop="1">
       <c r="A36" s="33">
         <v>67</v>
       </c>
-      <c r="B36" s="255" t="s">
+      <c r="B36" s="256" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="45">
@@ -11379,7 +11376,7 @@
       <c r="A37" s="34">
         <v>69</v>
       </c>
-      <c r="B37" s="256"/>
+      <c r="B37" s="257"/>
       <c r="C37" s="46">
         <v>2</v>
       </c>
@@ -11515,7 +11512,7 @@
       <c r="A38" s="34">
         <v>71</v>
       </c>
-      <c r="B38" s="257"/>
+      <c r="B38" s="258"/>
       <c r="C38" s="46">
         <v>3</v>
       </c>
@@ -11651,7 +11648,7 @@
       <c r="A39" s="34">
         <v>73</v>
       </c>
-      <c r="B39" s="251"/>
+      <c r="B39" s="259"/>
       <c r="C39" s="46">
         <v>4</v>
       </c>
@@ -11785,7 +11782,7 @@
       <c r="A40" s="34">
         <v>75</v>
       </c>
-      <c r="B40" s="252"/>
+      <c r="B40" s="260"/>
       <c r="C40" s="46">
         <v>5</v>
       </c>
@@ -11925,7 +11922,7 @@
       <c r="A41" s="34">
         <v>77</v>
       </c>
-      <c r="B41" s="252"/>
+      <c r="B41" s="260"/>
       <c r="C41" s="46">
         <v>6</v>
       </c>
@@ -12061,7 +12058,7 @@
       <c r="A42" s="34">
         <v>79</v>
       </c>
-      <c r="B42" s="253"/>
+      <c r="B42" s="261"/>
       <c r="C42" s="48">
         <v>7</v>
       </c>
@@ -12195,17 +12192,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B28:B30"/>
     <mergeCell ref="B39:B42"/>
     <mergeCell ref="B31:B35"/>
     <mergeCell ref="B23:B27"/>
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="B15:B19"/>
     <mergeCell ref="B36:B38"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B28:B30"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="BB1:BC1">

</xml_diff>

<commit_message>
Added read numbers and md5
</commit_message>
<xml_diff>
--- a/scripts/projects/under_ice/meta_data.xlsx
+++ b/scripts/projects/under_ice/meta_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="371">
   <si>
     <t>Sample</t>
   </si>
@@ -994,6 +994,144 @@
   </si>
   <si>
     <t>kt8</t>
+  </si>
+  <si>
+    <t>0636ef5852867394ec3e54a8afa578f4</t>
+  </si>
+  <si>
+    <t>5c54b0f9afccc785170d9ca06e7afff0</t>
+  </si>
+  <si>
+    <t>1dafd4352d7b1880d6878f5885f8aaba</t>
+  </si>
+  <si>
+    <t>87e5e1d5cfdd2c8ba72f9283164403ff</t>
+  </si>
+  <si>
+    <t>a4624e19657b1e221f464de9ae8487ea</t>
+  </si>
+  <si>
+    <t>36bd7d08f530bf11815be767908844dc</t>
+  </si>
+  <si>
+    <t>1c5ea01efecd43463923f6996ac58b7b</t>
+  </si>
+  <si>
+    <t>acdfb9f813a1236ad558b1a44d24ef8d</t>
+  </si>
+  <si>
+    <t>739f102045646ceafd74994d7ad817e6</t>
+  </si>
+  <si>
+    <t>d8b77993889b8b7b38a9c3422155e114</t>
+  </si>
+  <si>
+    <t>e11fee38f106403b60096dd7e6ed0365</t>
+  </si>
+  <si>
+    <t>b10069c19d0eeb6810340f1edacd5dd3</t>
+  </si>
+  <si>
+    <t>509a35321d2f473d85c5aeebec04ba78</t>
+  </si>
+  <si>
+    <t>14dc42f8bb66c71c42e54ca14615ab10</t>
+  </si>
+  <si>
+    <t>6e8b3f3def78cca3e73707e4cbc3dd4f</t>
+  </si>
+  <si>
+    <t>a617a75ce575a430b87737eb0c79ad24</t>
+  </si>
+  <si>
+    <t>5df9023d43755d7da14730b104071acf</t>
+  </si>
+  <si>
+    <t>8ebeacd8918d989e7455532c2313f8e5</t>
+  </si>
+  <si>
+    <t>2b8ecfd1f47277d285debe44f50cc254</t>
+  </si>
+  <si>
+    <t>66c1a02b76aa49366fbbb4033d938d1e</t>
+  </si>
+  <si>
+    <t>a99e0415a5c3686cf3f339549d4ca6c2</t>
+  </si>
+  <si>
+    <t>c039a8b29dfc2a98b3b6abae7f7457d4</t>
+  </si>
+  <si>
+    <t>da02dd872eaa353d4affd00e50c22cf4</t>
+  </si>
+  <si>
+    <t>bc085f44e0290d6909130ffd900181f4</t>
+  </si>
+  <si>
+    <t>59dfd4fcfd12e17c2096672335956f7d</t>
+  </si>
+  <si>
+    <t>9fd1f06db52427c4ce462aa8e4e47f27</t>
+  </si>
+  <si>
+    <t>a523929a72814e255bddfead0d6528d6</t>
+  </si>
+  <si>
+    <t>b72840cf821f742963c074629f0293c2</t>
+  </si>
+  <si>
+    <t>fabafcac86e29515c4cfc3203b1fd1d3</t>
+  </si>
+  <si>
+    <t>47c59ac78d38568c7a7bd5d6cecc6776</t>
+  </si>
+  <si>
+    <t>af10e84d49499252ecd23701cff9ab03</t>
+  </si>
+  <si>
+    <t>fef8f102eea7eb6d388aaae6caac0552</t>
+  </si>
+  <si>
+    <t>865136a19942b98742ea5e5d681b03ee</t>
+  </si>
+  <si>
+    <t>16379bb903f026bcadeb7990a8eadbdf</t>
+  </si>
+  <si>
+    <t>ea2fd05e14905888002dc0ffc9ec15bd</t>
+  </si>
+  <si>
+    <t>26847b246848562fb4079851726fc9cc</t>
+  </si>
+  <si>
+    <t>08ab0caab00e4913f39cc7f72076c10b</t>
+  </si>
+  <si>
+    <t>095e003effc78d1e7de139dd1c1c6d65</t>
+  </si>
+  <si>
+    <t>bf40092766421a768e60162e4b9f2780</t>
+  </si>
+  <si>
+    <t>e31d94363d917838001c3b2aa9fecb9a</t>
+  </si>
+  <si>
+    <t>528b9da8d0e122be4a6cf9c5e37a80ff</t>
+  </si>
+  <si>
+    <t>8fac7e60e35c2d278563322df43fe94e</t>
+  </si>
+  <si>
+    <t>504ea208c80af4b8c080fa7cc0680a03</t>
+  </si>
+  <si>
+    <t>d71b12045fa10a5b88ae7b19d2e34692</t>
+  </si>
+  <si>
+    <t>eafe11f52e0c90a5d04e8b0ad8f68459</t>
+  </si>
+  <si>
+    <t>1e6a73716100044b8f7555a1e0d137e1</t>
   </si>
 </sst>
 </file>
@@ -2232,13 +2370,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3076,7 +3220,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3096,6 +3240,8 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
@@ -3509,10 +3655,10 @@
   <dimension ref="A1:CL43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="CD2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AV2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BP38" sqref="BP38"/>
+      <selection pane="bottomRight" activeCell="BC34" sqref="BC34:BC35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5269,10 +5415,18 @@
       <c r="BA12" s="223" t="s">
         <v>237</v>
       </c>
-      <c r="BB12" s="223"/>
-      <c r="BC12" s="223"/>
-      <c r="BD12" s="223"/>
-      <c r="BE12" s="223"/>
+      <c r="BB12" s="223">
+        <v>8661770</v>
+      </c>
+      <c r="BC12" s="223">
+        <v>8661770</v>
+      </c>
+      <c r="BD12" s="223" t="s">
+        <v>325</v>
+      </c>
+      <c r="BE12" s="223" t="s">
+        <v>348</v>
+      </c>
       <c r="BF12" s="224" t="s">
         <v>270</v>
       </c>
@@ -5528,10 +5682,18 @@
       <c r="BA13" s="223" t="s">
         <v>239</v>
       </c>
-      <c r="BB13" s="223"/>
-      <c r="BC13" s="223"/>
-      <c r="BD13" s="223"/>
-      <c r="BE13" s="223"/>
+      <c r="BB13" s="223">
+        <v>10896437</v>
+      </c>
+      <c r="BC13" s="223">
+        <v>10896437</v>
+      </c>
+      <c r="BD13" s="223" t="s">
+        <v>326</v>
+      </c>
+      <c r="BE13" s="223" t="s">
+        <v>349</v>
+      </c>
       <c r="BF13" s="224" t="s">
         <v>270</v>
       </c>
@@ -5785,10 +5947,18 @@
       <c r="BA14" s="223" t="s">
         <v>241</v>
       </c>
-      <c r="BB14" s="223"/>
-      <c r="BC14" s="223"/>
-      <c r="BD14" s="223"/>
-      <c r="BE14" s="223"/>
+      <c r="BB14" s="223">
+        <v>5060871</v>
+      </c>
+      <c r="BC14" s="223">
+        <v>5060871</v>
+      </c>
+      <c r="BD14" s="223" t="s">
+        <v>327</v>
+      </c>
+      <c r="BE14" s="223" t="s">
+        <v>350</v>
+      </c>
       <c r="BF14" s="224" t="s">
         <v>270</v>
       </c>
@@ -6044,10 +6214,18 @@
       <c r="BA15" s="223" t="s">
         <v>243</v>
       </c>
-      <c r="BB15" s="223"/>
-      <c r="BC15" s="223"/>
-      <c r="BD15" s="223"/>
-      <c r="BE15" s="223"/>
+      <c r="BB15" s="223">
+        <v>6618705</v>
+      </c>
+      <c r="BC15" s="223">
+        <v>6618705</v>
+      </c>
+      <c r="BD15" s="223" t="s">
+        <v>328</v>
+      </c>
+      <c r="BE15" s="223" t="s">
+        <v>351</v>
+      </c>
       <c r="BF15" s="224" t="s">
         <v>270</v>
       </c>
@@ -6303,10 +6481,18 @@
       <c r="BA16" s="223" t="s">
         <v>245</v>
       </c>
-      <c r="BB16" s="223"/>
-      <c r="BC16" s="223"/>
-      <c r="BD16" s="223"/>
-      <c r="BE16" s="223"/>
+      <c r="BB16" s="223">
+        <v>7778364</v>
+      </c>
+      <c r="BC16" s="223">
+        <v>7778364</v>
+      </c>
+      <c r="BD16" s="223" t="s">
+        <v>329</v>
+      </c>
+      <c r="BE16" s="223" t="s">
+        <v>352</v>
+      </c>
       <c r="BF16" s="224" t="s">
         <v>270</v>
       </c>
@@ -6562,10 +6748,18 @@
       <c r="BA17" s="223" t="s">
         <v>247</v>
       </c>
-      <c r="BB17" s="223"/>
-      <c r="BC17" s="223"/>
-      <c r="BD17" s="223"/>
-      <c r="BE17" s="223"/>
+      <c r="BB17" s="223">
+        <v>6342961</v>
+      </c>
+      <c r="BC17" s="223">
+        <v>6342961</v>
+      </c>
+      <c r="BD17" s="223" t="s">
+        <v>330</v>
+      </c>
+      <c r="BE17" s="223" t="s">
+        <v>353</v>
+      </c>
       <c r="BF17" s="224" t="s">
         <v>270</v>
       </c>
@@ -6821,10 +7015,18 @@
       <c r="BA18" s="223" t="s">
         <v>249</v>
       </c>
-      <c r="BB18" s="223"/>
-      <c r="BC18" s="223"/>
-      <c r="BD18" s="223"/>
-      <c r="BE18" s="223"/>
+      <c r="BB18" s="223">
+        <v>7719837</v>
+      </c>
+      <c r="BC18" s="223">
+        <v>7719837</v>
+      </c>
+      <c r="BD18" s="223" t="s">
+        <v>331</v>
+      </c>
+      <c r="BE18" s="223" t="s">
+        <v>354</v>
+      </c>
       <c r="BF18" s="224" t="s">
         <v>270</v>
       </c>
@@ -7080,10 +7282,18 @@
       <c r="BA19" s="223" t="s">
         <v>251</v>
       </c>
-      <c r="BB19" s="223"/>
-      <c r="BC19" s="223"/>
-      <c r="BD19" s="223"/>
-      <c r="BE19" s="223"/>
+      <c r="BB19" s="223">
+        <v>7173828</v>
+      </c>
+      <c r="BC19" s="223">
+        <v>7173828</v>
+      </c>
+      <c r="BD19" s="223" t="s">
+        <v>332</v>
+      </c>
+      <c r="BE19" s="223" t="s">
+        <v>355</v>
+      </c>
       <c r="BF19" s="224" t="s">
         <v>270</v>
       </c>
@@ -7341,10 +7551,18 @@
       <c r="BA20" s="223" t="s">
         <v>253</v>
       </c>
-      <c r="BB20" s="223"/>
-      <c r="BC20" s="223"/>
-      <c r="BD20" s="223"/>
-      <c r="BE20" s="223"/>
+      <c r="BB20" s="223">
+        <v>6425591</v>
+      </c>
+      <c r="BC20" s="223">
+        <v>6425591</v>
+      </c>
+      <c r="BD20" s="223" t="s">
+        <v>333</v>
+      </c>
+      <c r="BE20" s="223" t="s">
+        <v>356</v>
+      </c>
       <c r="BF20" s="224" t="s">
         <v>270</v>
       </c>
@@ -7600,10 +7818,18 @@
       <c r="BA21" s="223" t="s">
         <v>255</v>
       </c>
-      <c r="BB21" s="223"/>
-      <c r="BC21" s="223"/>
-      <c r="BD21" s="223"/>
-      <c r="BE21" s="223"/>
+      <c r="BB21" s="223">
+        <v>8214080</v>
+      </c>
+      <c r="BC21" s="223">
+        <v>8214080</v>
+      </c>
+      <c r="BD21" s="223" t="s">
+        <v>334</v>
+      </c>
+      <c r="BE21" s="223" t="s">
+        <v>357</v>
+      </c>
       <c r="BF21" s="224" t="s">
         <v>270</v>
       </c>
@@ -7859,10 +8085,18 @@
       <c r="BA22" s="223" t="s">
         <v>257</v>
       </c>
-      <c r="BB22" s="223"/>
-      <c r="BC22" s="223"/>
-      <c r="BD22" s="223"/>
-      <c r="BE22" s="223"/>
+      <c r="BB22" s="223">
+        <v>7350565</v>
+      </c>
+      <c r="BC22" s="223">
+        <v>7350565</v>
+      </c>
+      <c r="BD22" s="223" t="s">
+        <v>335</v>
+      </c>
+      <c r="BE22" s="223" t="s">
+        <v>358</v>
+      </c>
       <c r="BF22" s="224" t="s">
         <v>270</v>
       </c>
@@ -8118,10 +8352,18 @@
       <c r="BA23" s="223" t="s">
         <v>259</v>
       </c>
-      <c r="BB23" s="223"/>
-      <c r="BC23" s="223"/>
-      <c r="BD23" s="223"/>
-      <c r="BE23" s="223"/>
+      <c r="BB23" s="223">
+        <v>7973836</v>
+      </c>
+      <c r="BC23" s="223">
+        <v>7973836</v>
+      </c>
+      <c r="BD23" s="223" t="s">
+        <v>336</v>
+      </c>
+      <c r="BE23" s="223" t="s">
+        <v>359</v>
+      </c>
       <c r="BF23" s="224" t="s">
         <v>270</v>
       </c>
@@ -8377,10 +8619,18 @@
       <c r="BA24" s="223" t="s">
         <v>261</v>
       </c>
-      <c r="BB24" s="223"/>
-      <c r="BC24" s="223"/>
-      <c r="BD24" s="223"/>
-      <c r="BE24" s="223"/>
+      <c r="BB24" s="223">
+        <v>7253125</v>
+      </c>
+      <c r="BC24" s="223">
+        <v>7253125</v>
+      </c>
+      <c r="BD24" s="223" t="s">
+        <v>337</v>
+      </c>
+      <c r="BE24" s="223" t="s">
+        <v>360</v>
+      </c>
       <c r="BF24" s="224" t="s">
         <v>270</v>
       </c>
@@ -8636,10 +8886,18 @@
       <c r="BA25" s="223" t="s">
         <v>263</v>
       </c>
-      <c r="BB25" s="223"/>
-      <c r="BC25" s="223"/>
-      <c r="BD25" s="223"/>
-      <c r="BE25" s="223"/>
+      <c r="BB25" s="223">
+        <v>7765627</v>
+      </c>
+      <c r="BC25" s="223">
+        <v>7765627</v>
+      </c>
+      <c r="BD25" s="223" t="s">
+        <v>338</v>
+      </c>
+      <c r="BE25" s="223" t="s">
+        <v>361</v>
+      </c>
       <c r="BF25" s="224" t="s">
         <v>270</v>
       </c>
@@ -8899,10 +9157,18 @@
       <c r="BA26" s="223" t="s">
         <v>265</v>
       </c>
-      <c r="BB26" s="223"/>
-      <c r="BC26" s="223"/>
-      <c r="BD26" s="223"/>
-      <c r="BE26" s="223"/>
+      <c r="BB26" s="223">
+        <v>8425739</v>
+      </c>
+      <c r="BC26" s="223">
+        <v>8425739</v>
+      </c>
+      <c r="BD26" s="223" t="s">
+        <v>339</v>
+      </c>
+      <c r="BE26" s="223" t="s">
+        <v>362</v>
+      </c>
       <c r="BF26" s="224" t="s">
         <v>270</v>
       </c>
@@ -9162,10 +9428,18 @@
       <c r="BA27" s="223" t="s">
         <v>267</v>
       </c>
-      <c r="BB27" s="223"/>
-      <c r="BC27" s="223"/>
-      <c r="BD27" s="223"/>
-      <c r="BE27" s="223"/>
+      <c r="BB27" s="223">
+        <v>8938420</v>
+      </c>
+      <c r="BC27" s="223">
+        <v>8938420</v>
+      </c>
+      <c r="BD27" s="223" t="s">
+        <v>340</v>
+      </c>
+      <c r="BE27" s="223" t="s">
+        <v>363</v>
+      </c>
       <c r="BF27" s="224" t="s">
         <v>270</v>
       </c>
@@ -9421,10 +9695,18 @@
       <c r="BA28" s="223" t="s">
         <v>223</v>
       </c>
-      <c r="BB28" s="223"/>
-      <c r="BC28" s="223"/>
-      <c r="BD28" s="223"/>
-      <c r="BE28" s="223"/>
+      <c r="BB28" s="223">
+        <v>8004303</v>
+      </c>
+      <c r="BC28" s="223">
+        <v>8004303</v>
+      </c>
+      <c r="BD28" s="223" t="s">
+        <v>341</v>
+      </c>
+      <c r="BE28" s="223" t="s">
+        <v>364</v>
+      </c>
       <c r="BF28" s="224" t="s">
         <v>270</v>
       </c>
@@ -9678,10 +9960,18 @@
       <c r="BA29" s="223" t="s">
         <v>225</v>
       </c>
-      <c r="BB29" s="223"/>
-      <c r="BC29" s="223"/>
-      <c r="BD29" s="223"/>
-      <c r="BE29" s="223"/>
+      <c r="BB29" s="223">
+        <v>8373052</v>
+      </c>
+      <c r="BC29" s="223">
+        <v>8373052</v>
+      </c>
+      <c r="BD29" s="223" t="s">
+        <v>342</v>
+      </c>
+      <c r="BE29" s="223" t="s">
+        <v>365</v>
+      </c>
       <c r="BF29" s="224" t="s">
         <v>270</v>
       </c>
@@ -9935,10 +10225,18 @@
       <c r="BA30" s="223" t="s">
         <v>227</v>
       </c>
-      <c r="BB30" s="223"/>
-      <c r="BC30" s="223"/>
-      <c r="BD30" s="223"/>
-      <c r="BE30" s="223"/>
+      <c r="BB30" s="223">
+        <v>8380324</v>
+      </c>
+      <c r="BC30" s="223">
+        <v>8380324</v>
+      </c>
+      <c r="BD30" s="223" t="s">
+        <v>343</v>
+      </c>
+      <c r="BE30" s="223" t="s">
+        <v>366</v>
+      </c>
       <c r="BF30" s="224" t="s">
         <v>270</v>
       </c>
@@ -10192,10 +10490,18 @@
       <c r="BA31" s="223" t="s">
         <v>229</v>
       </c>
-      <c r="BB31" s="223"/>
-      <c r="BC31" s="223"/>
-      <c r="BD31" s="223"/>
-      <c r="BE31" s="223"/>
+      <c r="BB31" s="223">
+        <v>7785774</v>
+      </c>
+      <c r="BC31" s="223">
+        <v>7785774</v>
+      </c>
+      <c r="BD31" s="223" t="s">
+        <v>344</v>
+      </c>
+      <c r="BE31" s="223" t="s">
+        <v>367</v>
+      </c>
       <c r="BF31" s="224" t="s">
         <v>270</v>
       </c>
@@ -10449,10 +10755,18 @@
       <c r="BA32" s="223" t="s">
         <v>231</v>
       </c>
-      <c r="BB32" s="223"/>
-      <c r="BC32" s="223"/>
-      <c r="BD32" s="223"/>
-      <c r="BE32" s="223"/>
+      <c r="BB32" s="223">
+        <v>7590249</v>
+      </c>
+      <c r="BC32" s="223">
+        <v>7590249</v>
+      </c>
+      <c r="BD32" s="223" t="s">
+        <v>345</v>
+      </c>
+      <c r="BE32" s="223" t="s">
+        <v>368</v>
+      </c>
       <c r="BF32" s="224" t="s">
         <v>270</v>
       </c>
@@ -10873,10 +11187,18 @@
       <c r="BA34" s="223" t="s">
         <v>233</v>
       </c>
-      <c r="BB34" s="223"/>
-      <c r="BC34" s="223"/>
-      <c r="BD34" s="223"/>
-      <c r="BE34" s="223"/>
+      <c r="BB34" s="223">
+        <v>7232302</v>
+      </c>
+      <c r="BC34" s="223">
+        <v>7232302</v>
+      </c>
+      <c r="BD34" s="223" t="s">
+        <v>346</v>
+      </c>
+      <c r="BE34" s="223" t="s">
+        <v>369</v>
+      </c>
       <c r="BF34" s="224" t="s">
         <v>270</v>
       </c>
@@ -11130,10 +11452,18 @@
       <c r="BA35" s="223" t="s">
         <v>235</v>
       </c>
-      <c r="BB35" s="223"/>
-      <c r="BC35" s="223"/>
-      <c r="BD35" s="223"/>
-      <c r="BE35" s="223"/>
+      <c r="BB35" s="223">
+        <v>8242886</v>
+      </c>
+      <c r="BC35" s="223">
+        <v>8242886</v>
+      </c>
+      <c r="BD35" s="223" t="s">
+        <v>347</v>
+      </c>
+      <c r="BE35" s="223" t="s">
+        <v>370</v>
+      </c>
       <c r="BF35" s="224" t="s">
         <v>270</v>
       </c>
@@ -12253,6 +12583,7 @@
     <hyperlink ref="AS42" r:id="rId40"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Excel file for soda_rerun
</commit_message>
<xml_diff>
--- a/scripts/projects/under_ice/meta_data.xlsx
+++ b/scripts/projects/under_ice/meta_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28720" windowHeight="16980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="SUMMARY.csv" sheetId="1" r:id="rId1"/>
@@ -3183,6 +3183,27 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="71" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3196,27 +3217,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="71" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3752,10 +3752,10 @@
       <c r="W1" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="251" t="s">
+      <c r="X1" s="258" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="252"/>
+      <c r="Y1" s="259"/>
       <c r="Z1" s="250" t="s">
         <v>323</v>
       </c>
@@ -4172,7 +4172,7 @@
       <c r="A4" s="33">
         <v>3</v>
       </c>
-      <c r="B4" s="256" t="s">
+      <c r="B4" s="255" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="45">
@@ -4310,7 +4310,7 @@
       <c r="A5" s="34">
         <v>5</v>
       </c>
-      <c r="B5" s="257"/>
+      <c r="B5" s="256"/>
       <c r="C5" s="46">
         <v>2</v>
       </c>
@@ -4446,7 +4446,7 @@
       <c r="A6" s="34">
         <v>7</v>
       </c>
-      <c r="B6" s="258"/>
+      <c r="B6" s="257"/>
       <c r="C6" s="46">
         <v>3</v>
       </c>
@@ -4582,7 +4582,7 @@
       <c r="A7" s="34">
         <v>9</v>
       </c>
-      <c r="B7" s="259"/>
+      <c r="B7" s="251"/>
       <c r="C7" s="46">
         <v>4</v>
       </c>
@@ -4718,7 +4718,7 @@
       <c r="A8" s="34">
         <v>11</v>
       </c>
-      <c r="B8" s="260"/>
+      <c r="B8" s="252"/>
       <c r="C8" s="46">
         <v>5</v>
       </c>
@@ -4854,7 +4854,7 @@
       <c r="A9" s="34">
         <v>13</v>
       </c>
-      <c r="B9" s="260"/>
+      <c r="B9" s="252"/>
       <c r="C9" s="46">
         <v>6</v>
       </c>
@@ -4990,7 +4990,7 @@
       <c r="A10" s="34">
         <v>15</v>
       </c>
-      <c r="B10" s="260"/>
+      <c r="B10" s="252"/>
       <c r="C10" s="46">
         <v>7</v>
       </c>
@@ -5126,7 +5126,7 @@
       <c r="A11" s="35">
         <v>17</v>
       </c>
-      <c r="B11" s="262"/>
+      <c r="B11" s="254"/>
       <c r="C11" s="47">
         <v>8</v>
       </c>
@@ -5262,7 +5262,7 @@
       <c r="A12" s="33">
         <v>19</v>
       </c>
-      <c r="B12" s="253" t="s">
+      <c r="B12" s="260" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="204">
@@ -5531,7 +5531,7 @@
       <c r="A13" s="34">
         <v>21</v>
       </c>
-      <c r="B13" s="254"/>
+      <c r="B13" s="261"/>
       <c r="C13" s="205">
         <v>2</v>
       </c>
@@ -5798,7 +5798,7 @@
       <c r="A14" s="34">
         <v>23</v>
       </c>
-      <c r="B14" s="255"/>
+      <c r="B14" s="262"/>
       <c r="C14" s="205">
         <v>3</v>
       </c>
@@ -6063,7 +6063,7 @@
       <c r="A15" s="34">
         <v>25</v>
       </c>
-      <c r="B15" s="259"/>
+      <c r="B15" s="251"/>
       <c r="C15" s="205">
         <v>4</v>
       </c>
@@ -6330,7 +6330,7 @@
       <c r="A16" s="34">
         <v>27</v>
       </c>
-      <c r="B16" s="260"/>
+      <c r="B16" s="252"/>
       <c r="C16" s="205">
         <v>5</v>
       </c>
@@ -6597,7 +6597,7 @@
       <c r="A17" s="34">
         <v>29</v>
       </c>
-      <c r="B17" s="260"/>
+      <c r="B17" s="252"/>
       <c r="C17" s="205">
         <v>6</v>
       </c>
@@ -6864,7 +6864,7 @@
       <c r="A18" s="34">
         <v>31</v>
       </c>
-      <c r="B18" s="260"/>
+      <c r="B18" s="252"/>
       <c r="C18" s="205">
         <v>7</v>
       </c>
@@ -7131,7 +7131,7 @@
       <c r="A19" s="35">
         <v>33</v>
       </c>
-      <c r="B19" s="262"/>
+      <c r="B19" s="254"/>
       <c r="C19" s="206">
         <v>8</v>
       </c>
@@ -7398,7 +7398,7 @@
       <c r="A20" s="33">
         <v>35</v>
       </c>
-      <c r="B20" s="256" t="s">
+      <c r="B20" s="255" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="204">
@@ -7667,7 +7667,7 @@
       <c r="A21" s="34">
         <v>37</v>
       </c>
-      <c r="B21" s="257"/>
+      <c r="B21" s="256"/>
       <c r="C21" s="207">
         <v>2</v>
       </c>
@@ -7934,7 +7934,7 @@
       <c r="A22" s="34">
         <v>39</v>
       </c>
-      <c r="B22" s="258"/>
+      <c r="B22" s="257"/>
       <c r="C22" s="207">
         <v>3</v>
       </c>
@@ -8201,7 +8201,7 @@
       <c r="A23" s="34">
         <v>41</v>
       </c>
-      <c r="B23" s="259"/>
+      <c r="B23" s="251"/>
       <c r="C23" s="205">
         <v>4</v>
       </c>
@@ -8468,7 +8468,7 @@
       <c r="A24" s="34">
         <v>43</v>
       </c>
-      <c r="B24" s="260"/>
+      <c r="B24" s="252"/>
       <c r="C24" s="205">
         <v>5</v>
       </c>
@@ -8735,7 +8735,7 @@
       <c r="A25" s="34">
         <v>45</v>
       </c>
-      <c r="B25" s="260"/>
+      <c r="B25" s="252"/>
       <c r="C25" s="205">
         <v>6</v>
       </c>
@@ -9002,7 +9002,7 @@
       <c r="A26" s="34">
         <v>47</v>
       </c>
-      <c r="B26" s="260"/>
+      <c r="B26" s="252"/>
       <c r="C26" s="205">
         <v>7</v>
       </c>
@@ -9273,7 +9273,7 @@
       <c r="A27" s="35">
         <v>49</v>
       </c>
-      <c r="B27" s="262"/>
+      <c r="B27" s="254"/>
       <c r="C27" s="206">
         <v>8</v>
       </c>
@@ -9544,7 +9544,7 @@
       <c r="A28" s="33">
         <v>51</v>
       </c>
-      <c r="B28" s="256" t="s">
+      <c r="B28" s="255" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="204">
@@ -9811,7 +9811,7 @@
       <c r="A29" s="34">
         <v>53</v>
       </c>
-      <c r="B29" s="257"/>
+      <c r="B29" s="256"/>
       <c r="C29" s="205">
         <v>2</v>
       </c>
@@ -10076,7 +10076,7 @@
       <c r="A30" s="34">
         <v>55</v>
       </c>
-      <c r="B30" s="258"/>
+      <c r="B30" s="257"/>
       <c r="C30" s="205">
         <v>3</v>
       </c>
@@ -10341,7 +10341,7 @@
       <c r="A31" s="34">
         <v>57</v>
       </c>
-      <c r="B31" s="259"/>
+      <c r="B31" s="251"/>
       <c r="C31" s="205">
         <v>4</v>
       </c>
@@ -10606,7 +10606,7 @@
       <c r="A32" s="34">
         <v>59</v>
       </c>
-      <c r="B32" s="260"/>
+      <c r="B32" s="252"/>
       <c r="C32" s="205">
         <v>5</v>
       </c>
@@ -10871,7 +10871,7 @@
       <c r="A33" s="34">
         <v>61</v>
       </c>
-      <c r="B33" s="260"/>
+      <c r="B33" s="252"/>
       <c r="C33" s="205">
         <v>6</v>
       </c>
@@ -11038,7 +11038,7 @@
       <c r="A34" s="34">
         <v>63</v>
       </c>
-      <c r="B34" s="260"/>
+      <c r="B34" s="252"/>
       <c r="C34" s="205">
         <v>7</v>
       </c>
@@ -11303,7 +11303,7 @@
       <c r="A35" s="35">
         <v>65</v>
       </c>
-      <c r="B35" s="262"/>
+      <c r="B35" s="254"/>
       <c r="C35" s="206">
         <v>8</v>
       </c>
@@ -11568,7 +11568,7 @@
       <c r="A36" s="33">
         <v>67</v>
       </c>
-      <c r="B36" s="256" t="s">
+      <c r="B36" s="255" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="45">
@@ -11706,7 +11706,7 @@
       <c r="A37" s="34">
         <v>69</v>
       </c>
-      <c r="B37" s="257"/>
+      <c r="B37" s="256"/>
       <c r="C37" s="46">
         <v>2</v>
       </c>
@@ -11842,7 +11842,7 @@
       <c r="A38" s="34">
         <v>71</v>
       </c>
-      <c r="B38" s="258"/>
+      <c r="B38" s="257"/>
       <c r="C38" s="46">
         <v>3</v>
       </c>
@@ -11978,7 +11978,7 @@
       <c r="A39" s="34">
         <v>73</v>
       </c>
-      <c r="B39" s="259"/>
+      <c r="B39" s="251"/>
       <c r="C39" s="46">
         <v>4</v>
       </c>
@@ -12112,7 +12112,7 @@
       <c r="A40" s="34">
         <v>75</v>
       </c>
-      <c r="B40" s="260"/>
+      <c r="B40" s="252"/>
       <c r="C40" s="46">
         <v>5</v>
       </c>
@@ -12252,7 +12252,7 @@
       <c r="A41" s="34">
         <v>77</v>
       </c>
-      <c r="B41" s="260"/>
+      <c r="B41" s="252"/>
       <c r="C41" s="46">
         <v>6</v>
       </c>
@@ -12388,7 +12388,7 @@
       <c r="A42" s="34">
         <v>79</v>
       </c>
-      <c r="B42" s="261"/>
+      <c r="B42" s="253"/>
       <c r="C42" s="48">
         <v>7</v>
       </c>
@@ -12522,17 +12522,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B28:B30"/>
     <mergeCell ref="B39:B42"/>
     <mergeCell ref="B31:B35"/>
     <mergeCell ref="B23:B27"/>
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="B15:B19"/>
     <mergeCell ref="B36:B38"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B28:B30"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="BB1:BC1">
@@ -12583,7 +12583,6 @@
     <hyperlink ref="AS42" r:id="rId40"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated under ice run numbers
</commit_message>
<xml_diff>
--- a/scripts/projects/under_ice/meta_data.xlsx
+++ b/scripts/projects/under_ice/meta_data.xlsx
@@ -2370,13 +2370,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3183,6 +3186,30 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3195,32 +3222,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="24">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3242,6 +3245,7 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
@@ -3655,10 +3659,10 @@
   <dimension ref="A1:CL43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AV2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="BN2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BC34" sqref="BC34:BC35"/>
+      <selection pane="bottomRight" activeCell="BO34" sqref="BO34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3752,10 +3756,10 @@
       <c r="W1" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="258" t="s">
+      <c r="X1" s="251" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="259"/>
+      <c r="Y1" s="252"/>
       <c r="Z1" s="250" t="s">
         <v>323</v>
       </c>
@@ -4172,7 +4176,7 @@
       <c r="A4" s="33">
         <v>3</v>
       </c>
-      <c r="B4" s="255" t="s">
+      <c r="B4" s="256" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="45">
@@ -4310,7 +4314,7 @@
       <c r="A5" s="34">
         <v>5</v>
       </c>
-      <c r="B5" s="256"/>
+      <c r="B5" s="257"/>
       <c r="C5" s="46">
         <v>2</v>
       </c>
@@ -4446,7 +4450,7 @@
       <c r="A6" s="34">
         <v>7</v>
       </c>
-      <c r="B6" s="257"/>
+      <c r="B6" s="258"/>
       <c r="C6" s="46">
         <v>3</v>
       </c>
@@ -4582,7 +4586,7 @@
       <c r="A7" s="34">
         <v>9</v>
       </c>
-      <c r="B7" s="251"/>
+      <c r="B7" s="259"/>
       <c r="C7" s="46">
         <v>4</v>
       </c>
@@ -4718,7 +4722,7 @@
       <c r="A8" s="34">
         <v>11</v>
       </c>
-      <c r="B8" s="252"/>
+      <c r="B8" s="260"/>
       <c r="C8" s="46">
         <v>5</v>
       </c>
@@ -4854,7 +4858,7 @@
       <c r="A9" s="34">
         <v>13</v>
       </c>
-      <c r="B9" s="252"/>
+      <c r="B9" s="260"/>
       <c r="C9" s="46">
         <v>6</v>
       </c>
@@ -4990,7 +4994,7 @@
       <c r="A10" s="34">
         <v>15</v>
       </c>
-      <c r="B10" s="252"/>
+      <c r="B10" s="260"/>
       <c r="C10" s="46">
         <v>7</v>
       </c>
@@ -5126,7 +5130,7 @@
       <c r="A11" s="35">
         <v>17</v>
       </c>
-      <c r="B11" s="254"/>
+      <c r="B11" s="262"/>
       <c r="C11" s="47">
         <v>8</v>
       </c>
@@ -5262,7 +5266,7 @@
       <c r="A12" s="33">
         <v>19</v>
       </c>
-      <c r="B12" s="260" t="s">
+      <c r="B12" s="253" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="204">
@@ -5531,7 +5535,7 @@
       <c r="A13" s="34">
         <v>21</v>
       </c>
-      <c r="B13" s="261"/>
+      <c r="B13" s="254"/>
       <c r="C13" s="205">
         <v>2</v>
       </c>
@@ -5798,7 +5802,7 @@
       <c r="A14" s="34">
         <v>23</v>
       </c>
-      <c r="B14" s="262"/>
+      <c r="B14" s="255"/>
       <c r="C14" s="205">
         <v>3</v>
       </c>
@@ -6063,7 +6067,7 @@
       <c r="A15" s="34">
         <v>25</v>
       </c>
-      <c r="B15" s="251"/>
+      <c r="B15" s="259"/>
       <c r="C15" s="205">
         <v>4</v>
       </c>
@@ -6330,7 +6334,7 @@
       <c r="A16" s="34">
         <v>27</v>
       </c>
-      <c r="B16" s="252"/>
+      <c r="B16" s="260"/>
       <c r="C16" s="205">
         <v>5</v>
       </c>
@@ -6597,7 +6601,7 @@
       <c r="A17" s="34">
         <v>29</v>
       </c>
-      <c r="B17" s="252"/>
+      <c r="B17" s="260"/>
       <c r="C17" s="205">
         <v>6</v>
       </c>
@@ -6864,7 +6868,7 @@
       <c r="A18" s="34">
         <v>31</v>
       </c>
-      <c r="B18" s="252"/>
+      <c r="B18" s="260"/>
       <c r="C18" s="205">
         <v>7</v>
       </c>
@@ -7131,7 +7135,7 @@
       <c r="A19" s="35">
         <v>33</v>
       </c>
-      <c r="B19" s="254"/>
+      <c r="B19" s="262"/>
       <c r="C19" s="206">
         <v>8</v>
       </c>
@@ -7398,7 +7402,7 @@
       <c r="A20" s="33">
         <v>35</v>
       </c>
-      <c r="B20" s="255" t="s">
+      <c r="B20" s="256" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="204">
@@ -7588,7 +7592,7 @@
         <v>156</v>
       </c>
       <c r="BN20" s="218">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BO20" s="222" t="s">
         <v>208</v>
@@ -7667,7 +7671,7 @@
       <c r="A21" s="34">
         <v>37</v>
       </c>
-      <c r="B21" s="256"/>
+      <c r="B21" s="257"/>
       <c r="C21" s="207">
         <v>2</v>
       </c>
@@ -7855,7 +7859,7 @@
         <v>156</v>
       </c>
       <c r="BN21" s="218">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BO21" s="222" t="s">
         <v>209</v>
@@ -7934,7 +7938,7 @@
       <c r="A22" s="34">
         <v>39</v>
       </c>
-      <c r="B22" s="257"/>
+      <c r="B22" s="258"/>
       <c r="C22" s="207">
         <v>3</v>
       </c>
@@ -8122,7 +8126,7 @@
         <v>156</v>
       </c>
       <c r="BN22" s="218">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BO22" s="222" t="s">
         <v>210</v>
@@ -8201,7 +8205,7 @@
       <c r="A23" s="34">
         <v>41</v>
       </c>
-      <c r="B23" s="251"/>
+      <c r="B23" s="259"/>
       <c r="C23" s="205">
         <v>4</v>
       </c>
@@ -8389,7 +8393,7 @@
         <v>156</v>
       </c>
       <c r="BN23" s="218">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BO23" s="222" t="s">
         <v>211</v>
@@ -8468,7 +8472,7 @@
       <c r="A24" s="34">
         <v>43</v>
       </c>
-      <c r="B24" s="252"/>
+      <c r="B24" s="260"/>
       <c r="C24" s="205">
         <v>5</v>
       </c>
@@ -8656,7 +8660,7 @@
         <v>156</v>
       </c>
       <c r="BN24" s="218">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BO24" s="222" t="s">
         <v>212</v>
@@ -8735,7 +8739,7 @@
       <c r="A25" s="34">
         <v>45</v>
       </c>
-      <c r="B25" s="252"/>
+      <c r="B25" s="260"/>
       <c r="C25" s="205">
         <v>6</v>
       </c>
@@ -8923,7 +8927,7 @@
         <v>156</v>
       </c>
       <c r="BN25" s="218">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BO25" s="222" t="s">
         <v>213</v>
@@ -9002,7 +9006,7 @@
       <c r="A26" s="34">
         <v>47</v>
       </c>
-      <c r="B26" s="252"/>
+      <c r="B26" s="260"/>
       <c r="C26" s="205">
         <v>7</v>
       </c>
@@ -9194,7 +9198,7 @@
         <v>156</v>
       </c>
       <c r="BN26" s="218">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BO26" s="222" t="s">
         <v>214</v>
@@ -9273,7 +9277,7 @@
       <c r="A27" s="35">
         <v>49</v>
       </c>
-      <c r="B27" s="254"/>
+      <c r="B27" s="262"/>
       <c r="C27" s="206">
         <v>8</v>
       </c>
@@ -9465,7 +9469,7 @@
         <v>156</v>
       </c>
       <c r="BN27" s="218">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BO27" s="222" t="s">
         <v>215</v>
@@ -9544,7 +9548,7 @@
       <c r="A28" s="33">
         <v>51</v>
       </c>
-      <c r="B28" s="255" t="s">
+      <c r="B28" s="256" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="204">
@@ -9732,7 +9736,7 @@
         <v>155</v>
       </c>
       <c r="BN28" s="218">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="BO28" s="222" t="s">
         <v>216</v>
@@ -9811,7 +9815,7 @@
       <c r="A29" s="34">
         <v>53</v>
       </c>
-      <c r="B29" s="256"/>
+      <c r="B29" s="257"/>
       <c r="C29" s="205">
         <v>2</v>
       </c>
@@ -9997,7 +10001,7 @@
         <v>155</v>
       </c>
       <c r="BN29" s="218">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="BO29" s="222" t="s">
         <v>217</v>
@@ -10076,7 +10080,7 @@
       <c r="A30" s="34">
         <v>55</v>
       </c>
-      <c r="B30" s="257"/>
+      <c r="B30" s="258"/>
       <c r="C30" s="205">
         <v>3</v>
       </c>
@@ -10262,7 +10266,7 @@
         <v>155</v>
       </c>
       <c r="BN30" s="218">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="BO30" s="222" t="s">
         <v>218</v>
@@ -10341,7 +10345,7 @@
       <c r="A31" s="34">
         <v>57</v>
       </c>
-      <c r="B31" s="251"/>
+      <c r="B31" s="259"/>
       <c r="C31" s="205">
         <v>4</v>
       </c>
@@ -10527,7 +10531,7 @@
         <v>155</v>
       </c>
       <c r="BN31" s="218">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="BO31" s="222" t="s">
         <v>219</v>
@@ -10606,7 +10610,7 @@
       <c r="A32" s="34">
         <v>59</v>
       </c>
-      <c r="B32" s="252"/>
+      <c r="B32" s="260"/>
       <c r="C32" s="205">
         <v>5</v>
       </c>
@@ -10792,7 +10796,7 @@
         <v>155</v>
       </c>
       <c r="BN32" s="218">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="BO32" s="222" t="s">
         <v>220</v>
@@ -10871,7 +10875,7 @@
       <c r="A33" s="34">
         <v>61</v>
       </c>
-      <c r="B33" s="252"/>
+      <c r="B33" s="260"/>
       <c r="C33" s="205">
         <v>6</v>
       </c>
@@ -11038,7 +11042,7 @@
       <c r="A34" s="34">
         <v>63</v>
       </c>
-      <c r="B34" s="252"/>
+      <c r="B34" s="260"/>
       <c r="C34" s="205">
         <v>7</v>
       </c>
@@ -11224,7 +11228,7 @@
         <v>155</v>
       </c>
       <c r="BN34" s="218">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="BO34" s="222" t="s">
         <v>221</v>
@@ -11303,7 +11307,7 @@
       <c r="A35" s="35">
         <v>65</v>
       </c>
-      <c r="B35" s="254"/>
+      <c r="B35" s="262"/>
       <c r="C35" s="206">
         <v>8</v>
       </c>
@@ -11489,7 +11493,7 @@
         <v>155</v>
       </c>
       <c r="BN35" s="218">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="BO35" s="222" t="s">
         <v>324</v>
@@ -11568,7 +11572,7 @@
       <c r="A36" s="33">
         <v>67</v>
       </c>
-      <c r="B36" s="255" t="s">
+      <c r="B36" s="256" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="45">
@@ -11706,7 +11710,7 @@
       <c r="A37" s="34">
         <v>69</v>
       </c>
-      <c r="B37" s="256"/>
+      <c r="B37" s="257"/>
       <c r="C37" s="46">
         <v>2</v>
       </c>
@@ -11842,7 +11846,7 @@
       <c r="A38" s="34">
         <v>71</v>
       </c>
-      <c r="B38" s="257"/>
+      <c r="B38" s="258"/>
       <c r="C38" s="46">
         <v>3</v>
       </c>
@@ -11978,7 +11982,7 @@
       <c r="A39" s="34">
         <v>73</v>
       </c>
-      <c r="B39" s="251"/>
+      <c r="B39" s="259"/>
       <c r="C39" s="46">
         <v>4</v>
       </c>
@@ -12112,7 +12116,7 @@
       <c r="A40" s="34">
         <v>75</v>
       </c>
-      <c r="B40" s="252"/>
+      <c r="B40" s="260"/>
       <c r="C40" s="46">
         <v>5</v>
       </c>
@@ -12252,7 +12256,7 @@
       <c r="A41" s="34">
         <v>77</v>
       </c>
-      <c r="B41" s="252"/>
+      <c r="B41" s="260"/>
       <c r="C41" s="46">
         <v>6</v>
       </c>
@@ -12388,7 +12392,7 @@
       <c r="A42" s="34">
         <v>79</v>
       </c>
-      <c r="B42" s="253"/>
+      <c r="B42" s="261"/>
       <c r="C42" s="48">
         <v>7</v>
       </c>
@@ -12522,17 +12526,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B28:B30"/>
     <mergeCell ref="B39:B42"/>
     <mergeCell ref="B31:B35"/>
     <mergeCell ref="B23:B27"/>
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="B15:B19"/>
     <mergeCell ref="B36:B38"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B28:B30"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="BB1:BC1">
@@ -12583,6 +12587,7 @@
     <hyperlink ref="AS42" r:id="rId40"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated under ice read length
</commit_message>
<xml_diff>
--- a/scripts/projects/under_ice/meta_data.xlsx
+++ b/scripts/projects/under_ice/meta_data.xlsx
@@ -2370,13 +2370,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3223,7 +3226,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="24">
+  <cellStyles count="25">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3246,6 +3249,7 @@
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
@@ -3662,7 +3666,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="BN2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BO34" sqref="BO34"/>
+      <selection pane="bottomRight" activeCell="CA33" sqref="CA33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5489,10 +5493,10 @@
         <v>302</v>
       </c>
       <c r="BY12" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ12" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA12" s="220" t="s">
         <v>303</v>
@@ -5756,10 +5760,10 @@
         <v>302</v>
       </c>
       <c r="BY13" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ13" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA13" s="220" t="s">
         <v>303</v>
@@ -6021,10 +6025,10 @@
         <v>302</v>
       </c>
       <c r="BY14" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ14" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA14" s="220" t="s">
         <v>303</v>
@@ -6288,10 +6292,10 @@
         <v>302</v>
       </c>
       <c r="BY15" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ15" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA15" s="220" t="s">
         <v>303</v>
@@ -6555,10 +6559,10 @@
         <v>302</v>
       </c>
       <c r="BY16" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ16" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA16" s="220" t="s">
         <v>303</v>
@@ -6822,10 +6826,10 @@
         <v>302</v>
       </c>
       <c r="BY17" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ17" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA17" s="220" t="s">
         <v>303</v>
@@ -7089,10 +7093,10 @@
         <v>302</v>
       </c>
       <c r="BY18" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ18" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA18" s="220" t="s">
         <v>303</v>
@@ -7356,10 +7360,10 @@
         <v>302</v>
       </c>
       <c r="BY19" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ19" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA19" s="220" t="s">
         <v>303</v>
@@ -7625,10 +7629,10 @@
         <v>302</v>
       </c>
       <c r="BY20" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ20" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA20" s="220" t="s">
         <v>303</v>
@@ -7892,10 +7896,10 @@
         <v>302</v>
       </c>
       <c r="BY21" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ21" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA21" s="220" t="s">
         <v>303</v>
@@ -8159,10 +8163,10 @@
         <v>302</v>
       </c>
       <c r="BY22" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ22" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA22" s="220" t="s">
         <v>303</v>
@@ -8426,10 +8430,10 @@
         <v>302</v>
       </c>
       <c r="BY23" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ23" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA23" s="220" t="s">
         <v>303</v>
@@ -8693,10 +8697,10 @@
         <v>302</v>
       </c>
       <c r="BY24" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ24" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA24" s="220" t="s">
         <v>303</v>
@@ -8960,10 +8964,10 @@
         <v>302</v>
       </c>
       <c r="BY25" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ25" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA25" s="220" t="s">
         <v>303</v>
@@ -9231,10 +9235,10 @@
         <v>302</v>
       </c>
       <c r="BY26" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ26" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA26" s="220" t="s">
         <v>303</v>
@@ -9502,10 +9506,10 @@
         <v>302</v>
       </c>
       <c r="BY27" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ27" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA27" s="220" t="s">
         <v>303</v>
@@ -9769,10 +9773,10 @@
         <v>302</v>
       </c>
       <c r="BY28" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ28" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA28" s="220" t="s">
         <v>303</v>
@@ -10034,10 +10038,10 @@
         <v>302</v>
       </c>
       <c r="BY29" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ29" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA29" s="220" t="s">
         <v>303</v>
@@ -10299,10 +10303,10 @@
         <v>302</v>
       </c>
       <c r="BY30" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ30" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA30" s="220" t="s">
         <v>303</v>
@@ -10564,10 +10568,10 @@
         <v>302</v>
       </c>
       <c r="BY31" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ31" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA31" s="220" t="s">
         <v>303</v>
@@ -10829,10 +10833,10 @@
         <v>302</v>
       </c>
       <c r="BY32" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ32" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA32" s="220" t="s">
         <v>303</v>
@@ -11261,10 +11265,10 @@
         <v>302</v>
       </c>
       <c r="BY34" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ34" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA34" s="220" t="s">
         <v>303</v>
@@ -11526,10 +11530,10 @@
         <v>302</v>
       </c>
       <c r="BY35" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ35" s="220">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA35" s="220" t="s">
         <v>303</v>

</xml_diff>